<commit_message>
August 2020 Measles Caseload Update
HR measles data ingest and about page changes for August 2020
</commit_message>
<xml_diff>
--- a/data-ingest/DRC/DRC_Measles_Caseload.xlsx
+++ b/data-ingest/DRC/DRC_Measles_Caseload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haile\Documents\GitHub\measles\data-ingest\DRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E400A43E-0829-425C-AB2A-18E98DB6D8AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B906F96-7129-45C3-9AD0-F88DBB18478F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4248" yWindow="0" windowWidth="10584" windowHeight="12960" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
+    <workbookView xWindow="6516" yWindow="3420" windowWidth="14964" windowHeight="9420" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
   <si>
     <t>reporting start date</t>
   </si>
@@ -477,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3E7FFC-8851-F442-B5D7-77C1AB79CDFE}">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1335,11 +1335,32 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="A40" s="7">
+        <v>43831</v>
+      </c>
+      <c r="B40" s="7">
+        <v>44052</v>
+      </c>
+      <c r="C40" s="3">
+        <v>69249</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1317</v>
+      </c>
+      <c r="E40" s="3">
+        <v>987</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40">
+        <f>SUM(C40-C39)</f>
+        <v>623</v>
+      </c>
+      <c r="H40">
+        <f>SUM(E40-E39)</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
@@ -1568,6 +1589,17 @@
         <v>49</v>
       </c>
     </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="1">
+        <v>623</v>
+      </c>
+      <c r="C66" s="1">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
September 20 - Measles Caseload Update
WHO Measles caseload update for data from September 2020
</commit_message>
<xml_diff>
--- a/data-ingest/DRC/DRC_Measles_Caseload.xlsx
+++ b/data-ingest/DRC/DRC_Measles_Caseload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haile\Documents\GitHub\measles\data-ingest\DRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B906F96-7129-45C3-9AD0-F88DBB18478F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E868C0B-0E96-43A7-8C6E-6B10CE48FC49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6516" yWindow="3420" windowWidth="14964" windowHeight="9420" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
+    <workbookView xWindow="4944" yWindow="1848" windowWidth="14964" windowHeight="9420" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
   <si>
     <t>reporting start date</t>
   </si>
@@ -477,9 +477,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3E7FFC-8851-F442-B5D7-77C1AB79CDFE}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
@@ -1363,11 +1363,32 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="A41" s="7">
+        <v>43831</v>
+      </c>
+      <c r="B41" s="7">
+        <v>44080</v>
+      </c>
+      <c r="C41" s="3">
+        <v>70899</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1317</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1026</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41">
+        <f>C41-C40</f>
+        <v>1650</v>
+      </c>
+      <c r="H41">
+        <f>E41-E40</f>
+        <v>39</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
@@ -1598,6 +1619,17 @@
       </c>
       <c r="C66" s="1">
         <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" s="1">
+        <v>1650</v>
+      </c>
+      <c r="C67" s="1">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
October 2021 measles caseload update
</commit_message>
<xml_diff>
--- a/data-ingest/DRC/DRC_Measles_Caseload.xlsx
+++ b/data-ingest/DRC/DRC_Measles_Caseload.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haile\Documents\GitHub\measles\data-ingest\DRC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorsborn/Documents/GitHub/measles/data-ingest/DRC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E868C0B-0E96-43A7-8C6E-6B10CE48FC49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D59218-FDDE-6043-89A6-3FF822125220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4944" yWindow="1848" windowWidth="14964" windowHeight="9420" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
+    <workbookView xWindow="3480" yWindow="500" windowWidth="32360" windowHeight="20100" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="32">
   <si>
     <t>reporting start date</t>
   </si>
@@ -96,16 +96,56 @@
   </si>
   <si>
     <t xml:space="preserve">January </t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Not reported</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -162,6 +202,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,22 +520,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3E7FFC-8851-F442-B5D7-77C1AB79CDFE}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="5" width="16.296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.796875" style="1"/>
+    <col min="4" max="5" width="16.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="13" max="14" width="11.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,8 +552,17 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>43466</v>
       </c>
@@ -528,8 +581,20 @@
       <c r="H2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>2019</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1">
+        <v>16254</v>
+      </c>
+      <c r="N2" s="1">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>43466</v>
       </c>
@@ -552,8 +617,17 @@
       <c r="H3" s="6">
         <v>284</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="1">
+        <v>13566</v>
+      </c>
+      <c r="N3" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>43466</v>
       </c>
@@ -566,8 +640,17 @@
       <c r="E4" s="1">
         <v>399</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>26622</v>
+      </c>
+      <c r="N4" s="1">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>43466</v>
       </c>
@@ -592,8 +675,17 @@
         <f>SUM(E5-E3)</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="1">
+        <v>19665</v>
+      </c>
+      <c r="N5" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>43466</v>
       </c>
@@ -618,8 +710,17 @@
         <f>SUM(E6-E5)</f>
         <v>439</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="1">
+        <v>30763</v>
+      </c>
+      <c r="N6" s="1">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>43466</v>
       </c>
@@ -632,8 +733,17 @@
       <c r="E7" s="1">
         <v>1129</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="1">
+        <v>11777</v>
+      </c>
+      <c r="N7" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>43466</v>
       </c>
@@ -647,8 +757,17 @@
       <c r="E8" s="3">
         <v>1181</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="1">
+        <v>36813</v>
+      </c>
+      <c r="N8" s="1">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>43466</v>
       </c>
@@ -673,8 +792,17 @@
         <f>SUM(E9-E6)</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="1">
+        <v>24017</v>
+      </c>
+      <c r="N9" s="1">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>43466</v>
       </c>
@@ -687,8 +815,17 @@
       <c r="E10" s="3">
         <v>1412</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="1">
+        <v>23702</v>
+      </c>
+      <c r="N10" s="1">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>43466</v>
       </c>
@@ -701,8 +838,17 @@
       <c r="E11" s="3">
         <v>1460</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="1">
+        <v>47091</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>43466</v>
       </c>
@@ -729,8 +875,17 @@
         <f>SUM(E12-E9)</f>
         <v>492</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="1">
+        <v>18809</v>
+      </c>
+      <c r="N12" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>43466</v>
       </c>
@@ -746,8 +901,17 @@
       <c r="E13" s="1">
         <v>1879</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="1">
+        <v>42392</v>
+      </c>
+      <c r="N13" s="1">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>43466</v>
       </c>
@@ -763,8 +927,20 @@
       <c r="E14" s="1">
         <v>1981</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K14">
+        <v>2020</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="1">
+        <v>18009</v>
+      </c>
+      <c r="N14" s="1">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>43466</v>
       </c>
@@ -791,8 +967,17 @@
         <f>SUM(E15-E12)</f>
         <v>246</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15" s="1">
+        <v>8565</v>
+      </c>
+      <c r="N15" s="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>43466</v>
       </c>
@@ -808,8 +993,17 @@
       <c r="E16" s="1">
         <v>2162</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="1">
+        <v>18544</v>
+      </c>
+      <c r="N16" s="1">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>43466</v>
       </c>
@@ -825,8 +1019,17 @@
       <c r="E17" s="1">
         <v>2581</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" s="1">
+        <v>10946</v>
+      </c>
+      <c r="N17" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>43466</v>
       </c>
@@ -853,8 +1056,17 @@
         <f>SUM(E18-E15)</f>
         <v>892</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="1">
+        <v>5143</v>
+      </c>
+      <c r="N18" s="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>43466</v>
       </c>
@@ -870,8 +1082,17 @@
       <c r="E19" s="1">
         <v>3006</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="1">
+        <v>3797</v>
+      </c>
+      <c r="N19" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>43466</v>
       </c>
@@ -887,8 +1108,17 @@
       <c r="E20" s="1">
         <v>3222</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="1">
+        <v>3622</v>
+      </c>
+      <c r="N20" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>43466</v>
       </c>
@@ -915,8 +1145,17 @@
         <f>SUM(E21-E18)</f>
         <v>606</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M21" s="1">
+        <v>623</v>
+      </c>
+      <c r="N21" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>43466</v>
       </c>
@@ -932,8 +1171,17 @@
       <c r="E22" s="1">
         <v>3559</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1650</v>
+      </c>
+      <c r="N22" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>43466</v>
       </c>
@@ -960,8 +1208,17 @@
         <f>SUM(E23-E21)</f>
         <v>506</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>43466</v>
       </c>
@@ -977,8 +1234,17 @@
       <c r="E24" s="1">
         <v>4189</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>43466</v>
       </c>
@@ -994,8 +1260,17 @@
       <c r="E25" s="1">
         <v>4455</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>43466</v>
       </c>
@@ -1011,8 +1286,20 @@
       <c r="E26" s="1">
         <v>4723</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>2021</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>43466</v>
       </c>
@@ -1039,8 +1326,17 @@
         <f>SUM(E27-E23)</f>
         <v>1045</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>43466</v>
       </c>
@@ -1065,8 +1361,17 @@
         <f>SUM(E28-E27)</f>
         <v>320</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>43466</v>
       </c>
@@ -1082,8 +1387,17 @@
       <c r="E29" s="1">
         <v>5604</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>43466</v>
       </c>
@@ -1099,8 +1413,17 @@
       <c r="E30" s="1">
         <v>5877</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>43466</v>
       </c>
@@ -1127,8 +1450,17 @@
         <f>SUM(E31-E28)</f>
         <v>615</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>43831</v>
       </c>
@@ -1151,8 +1483,17 @@
       <c r="H32" s="6">
         <v>221</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>43831</v>
       </c>
@@ -1176,8 +1517,17 @@
         <f>SUM(E33-E32)</f>
         <v>137</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>43831</v>
       </c>
@@ -1193,8 +1543,17 @@
       <c r="E34" s="1">
         <v>473</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>43831</v>
       </c>
@@ -1221,8 +1580,17 @@
         <f>SUM(E35-E33)</f>
         <v>216</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M35" s="1">
+        <v>47844</v>
+      </c>
+      <c r="N35" s="1">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>43831</v>
       </c>
@@ -1249,8 +1617,11 @@
         <f>SUM(E36-E35)</f>
         <v>146</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L36" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>43831</v>
       </c>
@@ -1277,8 +1648,11 @@
         <f>SUM(E37-E36)</f>
         <v>104</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L37" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>43831</v>
       </c>
@@ -1306,7 +1680,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>43831</v>
       </c>
@@ -1334,7 +1708,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>43831</v>
       </c>
@@ -1362,7 +1736,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>43831</v>
       </c>
@@ -1390,247 +1764,179 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>17</v>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
+        <v>43831</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="7">
+        <v>43831</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
+        <v>43831</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
+        <v>44197</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
+        <v>44197</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" s="1">
-        <v>16254</v>
-      </c>
-      <c r="C47" s="1">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="1">
-        <v>13566</v>
-      </c>
-      <c r="C48" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" s="1">
-        <v>26622</v>
-      </c>
-      <c r="C49" s="1">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B50" s="1">
-        <v>19665</v>
-      </c>
-      <c r="C50" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
+        <v>44197</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="7">
+        <v>44197</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="7">
+        <v>44197</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="1">
-        <v>30763</v>
-      </c>
-      <c r="C51" s="1">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="C49" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="7">
+        <v>44197</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="1">
-        <v>11777</v>
-      </c>
-      <c r="C52" s="1">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="C50" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="7">
+        <v>44197</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="1">
-        <v>36813</v>
-      </c>
-      <c r="C53" s="1">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B54" s="1">
-        <v>24017</v>
+      <c r="C51" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="7">
+        <v>44197</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="7">
+        <v>44197</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="7">
+        <v>44197</v>
+      </c>
+      <c r="B54" s="4">
+        <v>44479</v>
       </c>
       <c r="C54" s="1">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" s="1">
-        <v>23702</v>
+        <v>43277</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1113</v>
+      </c>
+      <c r="E54" s="1">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="9">
+        <v>44348</v>
+      </c>
+      <c r="B55" s="4">
+        <v>44486</v>
       </c>
       <c r="C55" s="1">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" s="1">
-        <v>47091</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" s="1">
-        <v>18809</v>
-      </c>
-      <c r="C57" s="1">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B58" s="1">
-        <v>42392</v>
-      </c>
-      <c r="C58" s="1">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B59" s="1">
-        <v>18009</v>
-      </c>
-      <c r="C59" s="1">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B60" s="1">
-        <v>8565</v>
-      </c>
-      <c r="C60" s="1">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B61" s="1">
-        <v>18544</v>
-      </c>
-      <c r="C61" s="1">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B62" s="1">
-        <v>10946</v>
-      </c>
-      <c r="C62" s="1">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B63" s="1">
-        <v>5143</v>
-      </c>
-      <c r="C63" s="1">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B64" s="1">
-        <v>3797</v>
-      </c>
-      <c r="C64" s="1">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B65" s="1">
-        <v>3622</v>
-      </c>
-      <c r="C65" s="1">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B66" s="1">
-        <v>623</v>
-      </c>
-      <c r="C66" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B67" s="1">
-        <v>1650</v>
-      </c>
-      <c r="C67" s="1">
-        <v>39</v>
-      </c>
+        <v>47844</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1193</v>
+      </c>
+      <c r="E55" s="1">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="9"/>
+      <c r="B56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="9"/>
+      <c r="B57" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WHO Measles Update - Nov 2021
Updating data for November 2021
</commit_message>
<xml_diff>
--- a/data-ingest/DRC/DRC_Measles_Caseload.xlsx
+++ b/data-ingest/DRC/DRC_Measles_Caseload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorsborn/Documents/GitHub/measles/data-ingest/DRC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haileyrobertson/Documents/GitHub/measles/data-ingest/DRC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D59218-FDDE-6043-89A6-3FF822125220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBFA1EB-77B2-514F-8981-534D1639E6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="500" windowWidth="32360" windowHeight="20100" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
+    <workbookView xWindow="16600" yWindow="500" windowWidth="19240" windowHeight="20100" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3E7FFC-8851-F442-B5D7-77C1AB79CDFE}">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1620,6 +1620,14 @@
       <c r="L36" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="M36" s="1">
+        <f>C56-C55</f>
+        <v>8096</v>
+      </c>
+      <c r="N36" s="1">
+        <f>E56-E55</f>
+        <v>131</v>
+      </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
@@ -1931,8 +1939,21 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="9"/>
-      <c r="B56" s="4"/>
+      <c r="A56" s="9">
+        <v>44348</v>
+      </c>
+      <c r="B56" s="4">
+        <v>44514</v>
+      </c>
+      <c r="C56" s="1">
+        <v>55940</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1193</v>
+      </c>
+      <c r="E56" s="1">
+        <v>825</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="9"/>

</xml_diff>

<commit_message>
February 2022 Measles Update
Feb 2022 update for data from Jan 2022
</commit_message>
<xml_diff>
--- a/data-ingest/DRC/DRC_Measles_Caseload.xlsx
+++ b/data-ingest/DRC/DRC_Measles_Caseload.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorsborn/Documents/GitHub/measles/data-ingest/DRC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haileyrobertson/Documents/GitHub/measles/data-ingest/DRC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6AAEF4-5B77-DB4E-8836-55145FFB9167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5302FCCB-1D1D-E64C-A87D-512738AC47F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39500" yWindow="-5900" windowWidth="35140" windowHeight="20100" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="35140" windowHeight="20100" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="23">
   <si>
     <t>reporting start date</t>
   </si>
@@ -98,34 +98,7 @@
     <t xml:space="preserve">January </t>
   </si>
   <si>
-    <t>Oct</t>
-  </si>
-  <si>
-    <t>Nov</t>
-  </si>
-  <si>
-    <t>Dec</t>
-  </si>
-  <si>
     <t>Not reported</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>Mar</t>
-  </si>
-  <si>
-    <t>Apr</t>
-  </si>
-  <si>
-    <t>Aug</t>
-  </si>
-  <si>
-    <t>Sep</t>
   </si>
   <si>
     <t>NA</t>
@@ -177,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -204,6 +177,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -520,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3E7FFC-8851-F442-B5D7-77C1AB79CDFE}">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1212,10 +1188,10 @@
         <v>14</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -1238,10 +1214,10 @@
         <v>16</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -1264,10 +1240,10 @@
         <v>15</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -1293,10 +1269,10 @@
         <v>5</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -1330,10 +1306,10 @@
         <v>6</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -1365,10 +1341,10 @@
         <v>7</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -1391,10 +1367,10 @@
         <v>8</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -1417,10 +1393,10 @@
         <v>9</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -1454,10 +1430,10 @@
         <v>10</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -1487,10 +1463,10 @@
         <v>11</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
@@ -1521,10 +1497,10 @@
         <v>12</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -1547,10 +1523,10 @@
         <v>13</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
@@ -1693,6 +1669,18 @@
         <f>SUM(E38-E37)</f>
         <v>95</v>
       </c>
+      <c r="K38">
+        <v>2022</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
@@ -1782,132 +1770,132 @@
       <c r="A42" s="7">
         <v>43831</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="10">
+        <v>44105</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>43831</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>22</v>
+      <c r="B43" s="10">
+        <v>44136</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>43831</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>23</v>
+      <c r="B44" s="10">
+        <v>44166</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>44197</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>25</v>
+      <c r="B45" s="10">
+        <v>44197</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>44197</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>26</v>
+      <c r="B46" s="10">
+        <v>44228</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>44197</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>27</v>
+      <c r="B47" s="10">
+        <v>44256</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>44197</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>28</v>
+      <c r="B48" s="10">
+        <v>44287</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>44197</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>9</v>
+      <c r="B49" s="10">
+        <v>44317</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>44197</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>10</v>
+      <c r="B50" s="10">
+        <v>44348</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>44197</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>11</v>
+      <c r="B51" s="10">
+        <v>44378</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>44197</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>29</v>
+      <c r="B52" s="10">
+        <v>44409</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>44197</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>30</v>
+      <c r="B53" s="10">
+        <v>44440</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1976,6 +1964,17 @@
       </c>
       <c r="E57" s="1">
         <v>825</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
+        <v>44348</v>
+      </c>
+      <c r="B58" s="10">
+        <v>44562</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-Run February 2022 Measles Update
Data from the month of January was changed retroactively. Database was cleared of previous values and update was completed with latest data.
</commit_message>
<xml_diff>
--- a/data-ingest/DRC/DRC_Measles_Caseload.xlsx
+++ b/data-ingest/DRC/DRC_Measles_Caseload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haileyrobertson/Documents/GitHub/measles/data-ingest/DRC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5302FCCB-1D1D-E64C-A87D-512738AC47F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63799CAC-C234-FA4E-A5F6-C5A53E0166BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="35140" windowHeight="20100" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="23">
   <si>
     <t>reporting start date</t>
   </si>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3E7FFC-8851-F442-B5D7-77C1AB79CDFE}">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1675,11 +1675,11 @@
       <c r="L38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>22</v>
+      <c r="M38" s="1">
+        <v>8379</v>
+      </c>
+      <c r="N38" s="1">
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
@@ -1968,13 +1968,19 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
-        <v>44348</v>
-      </c>
-      <c r="B58" s="10">
         <v>44562</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>21</v>
+      <c r="B58" s="4">
+        <v>44598</v>
+      </c>
+      <c r="C58" s="1">
+        <v>8379</v>
+      </c>
+      <c r="D58" s="1">
+        <v>142</v>
+      </c>
+      <c r="E58" s="1">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data for March 2022
Data for February 2022 was ingested into the site. Note: Only 46 countries are reporting data for this month.
</commit_message>
<xml_diff>
--- a/data-ingest/DRC/DRC_Measles_Caseload.xlsx
+++ b/data-ingest/DRC/DRC_Measles_Caseload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haileyrobertson/Documents/GitHub/measles/data-ingest/DRC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63799CAC-C234-FA4E-A5F6-C5A53E0166BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72078737-7C54-2644-9BA5-92976B74D14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="35140" windowHeight="20100" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="23">
   <si>
     <t>reporting start date</t>
   </si>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3E7FFC-8851-F442-B5D7-77C1AB79CDFE}">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1709,6 +1709,17 @@
         <f>E39-E38</f>
         <v>49</v>
       </c>
+      <c r="L39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M39" s="1">
+        <f>C59-C58</f>
+        <v>4810</v>
+      </c>
+      <c r="N39" s="1">
+        <f>E59-E58</f>
+        <v>114</v>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
@@ -1981,6 +1992,23 @@
       </c>
       <c r="E58" s="1">
         <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
+        <v>44562</v>
+      </c>
+      <c r="B59" s="4">
+        <v>44612</v>
+      </c>
+      <c r="C59" s="1">
+        <v>13189</v>
+      </c>
+      <c r="D59" s="1">
+        <v>338</v>
+      </c>
+      <c r="E59" s="1">
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete March 2022 data update
</commit_message>
<xml_diff>
--- a/data-ingest/DRC/DRC_Measles_Caseload.xlsx
+++ b/data-ingest/DRC/DRC_Measles_Caseload.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haileyrobertson/Documents/GitHub/measles/data-ingest/DRC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72078737-7C54-2644-9BA5-92976B74D14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665834A6-CAED-974B-80D6-F1789050991C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="35140" windowHeight="20100" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
+    <workbookView xWindow="37620" yWindow="1300" windowWidth="35140" windowHeight="19660" xr2:uid="{5AAA1D91-6338-8D40-8FE5-FCE0E873CB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="23">
   <si>
     <t>reporting start date</t>
   </si>
@@ -496,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3E7FFC-8851-F442-B5D7-77C1AB79CDFE}">
-  <dimension ref="A1:N59"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1748,6 +1746,17 @@
         <f>SUM(E40-E39)</f>
         <v>19</v>
       </c>
+      <c r="L40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M40" s="1">
+        <f>C60-C59</f>
+        <v>3960</v>
+      </c>
+      <c r="N40" s="1">
+        <f>E60-E59</f>
+        <v>76</v>
+      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
@@ -2009,6 +2018,23 @@
       </c>
       <c r="E59" s="1">
         <v>268</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
+        <v>44562</v>
+      </c>
+      <c r="B60" s="4">
+        <v>44626</v>
+      </c>
+      <c r="C60" s="1">
+        <v>17149</v>
+      </c>
+      <c r="D60" s="1">
+        <v>526</v>
+      </c>
+      <c r="E60" s="1">
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>